<commit_message>
Finished the excel files
</commit_message>
<xml_diff>
--- a/data/affinities.xlsx
+++ b/data/affinities.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -53,22 +53,22 @@
     <t>Cold</t>
   </si>
   <si>
+    <t>Causes frost buildup ()</t>
+  </si>
+  <si>
     <t>Poison</t>
   </si>
   <si>
+    <t>Causes poison buildup ()</t>
+  </si>
+  <si>
     <t>Blood</t>
   </si>
   <si>
+    <t>Causes blood loss buildup ()</t>
+  </si>
+  <si>
     <t>Occult</t>
-  </si>
-  <si>
-    <t>Causes frost buildup ()</t>
-  </si>
-  <si>
-    <t>Causes poison buildup ()</t>
-  </si>
-  <si>
-    <t>Causes blood loss buildup ()</t>
   </si>
 </sst>
 </file>
@@ -607,116 +607,77 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>1.0</v>
-      </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1">
-        <v>2.0</v>
-      </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1">
-        <v>3.0</v>
-      </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1">
-        <v>4.0</v>
-      </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1">
-        <v>5.0</v>
-      </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1">
-        <v>6.0</v>
-      </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1">
-        <v>7.0</v>
-      </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1">
-        <v>8.0</v>
-      </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1">
-        <v>9.0</v>
-      </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1">
-        <v>10.0</v>
-      </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1">
-        <v>1.0</v>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1">
-        <v>11.0</v>
-      </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2.0</v>
+        <v>14</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1">
-        <v>12.0</v>
-      </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1">
-        <v>3.0</v>
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1">
-        <v>13.0</v>
-      </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -821,31 +782,31 @@
         <v>12</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5"/>
       <c r="B12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8"/>
       <c r="B13" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="13"/>
       <c r="B14" s="14" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C14" s="15"/>
     </row>

</xml_diff>